<commit_message>
#ES-186 - added correlationId field in audit-logs-report-template.xlsx
</commit_message>
<xml_diff>
--- a/eca-report/src/main/resources/templates/audit-logs-report-template.xlsx
+++ b/eca-report/src/main/resources/templates/audit-logs-report-template.xlsx
@@ -46,7 +46,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="F8")</t>
+jx:area(lastCell="G8")</t>
         </r>
       </text>
     </comment>
@@ -70,7 +70,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:if(condition="not empty(report.searchQuery)", lastCell="F3", areas=["A3:B3"])</t>
+jx:if(condition="not empty(report.searchQuery)", lastCell="G3", areas=["A3:B3"])</t>
         </r>
       </text>
     </comment>
@@ -94,7 +94,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="report.filters" var="filter" lastCell="F4")</t>
+jx:each(items="report.filters" var="filter" lastCell="G4")</t>
         </r>
       </text>
     </comment>
@@ -118,7 +118,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="report.items" var="auditLog" lastCell="F7")</t>
+jx:each(items="report.items" var="auditLog" lastCell="G7")</t>
         </r>
       </text>
     </comment>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Строка поиска</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>${auditLog.codeTitle}</t>
+  </si>
+  <si>
+    <t>ID корреляции</t>
+  </si>
+  <si>
+    <t>${auditLog.correlationId}</t>
   </si>
 </sst>
 </file>
@@ -715,31 +721,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="43.6640625" customWidth="1"/>
     <col min="2" max="2" width="40.21875" customWidth="1"/>
-    <col min="3" max="3" width="56.77734375" customWidth="1"/>
-    <col min="4" max="4" width="61.109375" customWidth="1"/>
-    <col min="5" max="5" width="96.21875" customWidth="1"/>
-    <col min="6" max="7" width="32.33203125" customWidth="1"/>
-    <col min="8" max="8" width="51.88671875" customWidth="1"/>
-    <col min="9" max="9" width="57.77734375" customWidth="1"/>
-    <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="30.88671875" customWidth="1"/>
-    <col min="12" max="12" width="34.33203125" customWidth="1"/>
-    <col min="13" max="13" width="31.44140625" customWidth="1"/>
-    <col min="14" max="14" width="31.5546875" customWidth="1"/>
-    <col min="15" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="3" max="3" width="40.21875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="56.77734375" customWidth="1"/>
+    <col min="5" max="5" width="61.109375" customWidth="1"/>
+    <col min="6" max="6" width="96.21875" customWidth="1"/>
+    <col min="7" max="8" width="32.33203125" customWidth="1"/>
+    <col min="9" max="9" width="51.88671875" customWidth="1"/>
+    <col min="10" max="10" width="57.77734375" customWidth="1"/>
+    <col min="11" max="11" width="27" customWidth="1"/>
+    <col min="12" max="12" width="30.88671875" customWidth="1"/>
+    <col min="13" max="13" width="34.33203125" customWidth="1"/>
+    <col min="14" max="14" width="31.44140625" customWidth="1"/>
+    <col min="15" max="15" width="31.5546875" customWidth="1"/>
+    <col min="16" max="1026" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6">
+    <row r="1" spans="1:12" ht="15.6">
       <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
@@ -748,26 +755,28 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="16"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="15.6">
+    <row r="2" spans="1:12" ht="15.6">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="14.85" customHeight="1">
+    <row r="3" spans="1:12" ht="14.85" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -778,13 +787,14 @@
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="17"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="14.85" customHeight="1">
+    <row r="4" spans="1:12" ht="14.85" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -795,76 +805,84 @@
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1">
+    <row r="7" spans="1:12" ht="15" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" s="13" t="s">
         <v>4</v>
       </c>
@@ -872,19 +890,20 @@
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="11"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>